<commit_message>
Ran the latest version, adding all outputs
Final version seems to work great, no errors and much faster. Thanks
</commit_message>
<xml_diff>
--- a/output/Georgia/article1_Georgia.xlsx
+++ b/output/Georgia/article1_Georgia.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">segregation Battle of Normandy. </t>
+          <t xml:space="preserve">segregation </t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>477</v>
+        <v>524</v>
       </c>
       <c r="C2" t="n">
-        <v>690</v>
+        <v>644</v>
       </c>
       <c r="D2" t="n">
-        <v>280</v>
+        <v>103</v>
       </c>
       <c r="E2" t="n">
         <v>23</v>
@@ -482,17 +482,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">historically black college </t>
+          <t xml:space="preserve">Battle </t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>371</v>
+        <v>621</v>
       </c>
       <c r="C3" t="n">
-        <v>713</v>
+        <v>694</v>
       </c>
       <c r="D3" t="n">
-        <v>212</v>
+        <v>55</v>
       </c>
       <c r="E3" t="n">
         <v>23</v>
@@ -501,17 +501,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">school integration, </t>
+          <t xml:space="preserve">of </t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>572</v>
+        <v>676</v>
       </c>
       <c r="C4" t="n">
-        <v>1058</v>
+        <v>694</v>
       </c>
       <c r="D4" t="n">
-        <v>163</v>
+        <v>22</v>
       </c>
       <c r="E4" t="n">
         <v>23</v>
@@ -520,19 +520,209 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">civil rights activists </t>
+          <t xml:space="preserve">Normandy. </t>
         </is>
       </c>
       <c r="B5" t="n">
+        <v>698</v>
+      </c>
+      <c r="C5" t="n">
+        <v>694</v>
+      </c>
+      <c r="D5" t="n">
+        <v>102</v>
+      </c>
+      <c r="E5" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">historically </t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>477</v>
+      </c>
+      <c r="C6" t="n">
+        <v>719</v>
+      </c>
+      <c r="D6" t="n">
+        <v>99</v>
+      </c>
+      <c r="E6" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">black </t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>576</v>
+      </c>
+      <c r="C7" t="n">
+        <v>719</v>
+      </c>
+      <c r="D7" t="n">
+        <v>50</v>
+      </c>
+      <c r="E7" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">college </t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>626</v>
+      </c>
+      <c r="C8" t="n">
+        <v>719</v>
+      </c>
+      <c r="D8" t="n">
+        <v>63</v>
+      </c>
+      <c r="E8" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NAACP's </t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>477</v>
+      </c>
+      <c r="C9" t="n">
+        <v>968.1999999999999</v>
+      </c>
+      <c r="D9" t="n">
+        <v>82</v>
+      </c>
+      <c r="E9" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">boycotts </t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>397</v>
+      </c>
+      <c r="C10" t="n">
+        <v>993.1999999999999</v>
+      </c>
+      <c r="D10" t="n">
+        <v>76</v>
+      </c>
+      <c r="E10" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">school </t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>572</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1059.6</v>
+      </c>
+      <c r="D11" t="n">
+        <v>59</v>
+      </c>
+      <c r="E11" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">integration, </t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>631</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1059.6</v>
+      </c>
+      <c r="D12" t="n">
+        <v>104</v>
+      </c>
+      <c r="E12" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">civil </t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>268</v>
       </c>
-      <c r="C5" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D5" t="n">
-        <v>168</v>
-      </c>
-      <c r="E5" t="n">
+      <c r="C13" t="n">
+        <v>1151</v>
+      </c>
+      <c r="D13" t="n">
+        <v>40</v>
+      </c>
+      <c r="E13" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">rights </t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>308</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1151</v>
+      </c>
+      <c r="D14" t="n">
+        <v>54</v>
+      </c>
+      <c r="E14" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">activists </t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>362</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1151</v>
+      </c>
+      <c r="D15" t="n">
+        <v>74</v>
+      </c>
+      <c r="E15" t="n">
         <v>23</v>
       </c>
     </row>

</xml_diff>